<commit_message>
changes following Andrew's review rev0
</commit_message>
<xml_diff>
--- a/Matt_reqs.xlsx
+++ b/Matt_reqs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375CF291-BEBC-4901-81A5-2FC4A68A28BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E88E83-27EA-41AF-8295-560B0EEAABAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16810" yWindow="-3300" windowWidth="13640" windowHeight="15090" xr2:uid="{312FFB53-31D3-491C-8975-900746FDF726}"/>
+    <workbookView xWindow="-32850" yWindow="-4220" windowWidth="21450" windowHeight="13180" xr2:uid="{312FFB53-31D3-491C-8975-900746FDF726}"/>
   </bookViews>
   <sheets>
     <sheet name="FIFO" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Requirement Header</t>
   </si>
@@ -57,6 +57,9 @@
     <t>FIFO_INIT_01</t>
   </si>
   <si>
+    <t>FIFO_INIT_02</t>
+  </si>
+  <si>
     <t>Reset</t>
   </si>
   <si>
@@ -75,9 +78,6 @@
     <t>Module shall set o_empty flag logic high and o_full flag logic low upon system reset.</t>
   </si>
   <si>
-    <t>Module shall set parametrizable depth to (2,4,8 … 64) upon initialization.</t>
-  </si>
-  <si>
     <t>Module shall set the read and write pointers to all zeroes upon system reset.</t>
   </si>
   <si>
@@ -102,22 +102,28 @@
     <t>FIFO_R_02</t>
   </si>
   <si>
-    <t>Module shall write 128 bits of o_fifo_w_data to internal memory buffer when i_w_en is logic high.</t>
-  </si>
-  <si>
-    <t>Module shall set 128 bits of o_fifo_r_data to value of internal memory buffer when i_r_en is logic high.</t>
-  </si>
-  <si>
     <t>FIFO_R_03</t>
   </si>
   <si>
-    <t>Module shall set o_empty logic high when read pointer is equal to 1 less than the buffer length and write pointer is 0.</t>
-  </si>
-  <si>
-    <t>Module shall set o_full logic high when write pointer is equal to 1 less than the buffer length and read pointer is 0.</t>
-  </si>
-  <si>
     <t>IF</t>
+  </si>
+  <si>
+    <t>Module shall set FIFO_DEPTH to default 2 (optionally 2,4,8,16,32,64) upon initialization.</t>
+  </si>
+  <si>
+    <t>Module shall set o_full logic high when w_ptr is equal to 1 less than the buffer length and r_ptr is 0.</t>
+  </si>
+  <si>
+    <t>Module shall set o_empty logic high when r_ptr is equal to 1 less than the buffer length and w_ptr is 0.</t>
+  </si>
+  <si>
+    <t>Module shall include internal memory buffer mem_array to hold FIFO data</t>
+  </si>
+  <si>
+    <t>Module shall write 128 bits of o_fifo_w_data to mem_array[w_ptr] when i_w_en is logic high.</t>
+  </si>
+  <si>
+    <t>Module shall set 128 bits of o_fifo_r_data to value of mem_array[r_ptr] when i_r_en is logic high.</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -215,6 +221,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -344,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -356,55 +371,47 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D120AA-2BF7-423A-8400-39EB97BBCCF9}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,111 +758,122 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7" t="s">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="D11" s="13" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B10"/>
+  <mergeCells count="5">
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -893,8 +911,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>